<commit_message>
"html requests not working anymore"
</commit_message>
<xml_diff>
--- a/Attendance/f810.xlsx
+++ b/Attendance/f810.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="65">
   <si>
     <t xml:space="preserve">Név</t>
   </si>
@@ -49,6 +49,9 @@
     <t xml:space="preserve">Y3QFQK</t>
   </si>
   <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
     <t xml:space="preserve">336001084</t>
   </si>
   <si>
@@ -137,9 +140,6 @@
   </si>
   <si>
     <t xml:space="preserve">RUOCIU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0</t>
   </si>
   <si>
     <t xml:space="preserve">308185765</t>
@@ -221,9 +221,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -312,12 +313,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -329,11 +334,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -417,7 +422,7 @@
   <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -425,7 +430,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23"/>
@@ -444,369 +449,411 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="V1" s="3"/>
+      <c r="D1" s="2" t="n">
+        <v>43364</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="V1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="V2" s="3" t="s">
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="V2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="V3" s="3" t="s">
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>9</v>
       </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="V3" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="V4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="V4" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="V5" s="3" t="s">
+      <c r="B5" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="C5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="V5" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="V6" s="3" t="s">
+      <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="C6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="V6" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="V7" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="C7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="V7" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="V8" s="3" t="s">
+      <c r="B8" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="C8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="V8" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="V9" s="3" t="s">
+      <c r="B9" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="C9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="V9" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="V10" s="3" t="s">
+      <c r="B10" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="C10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="V10" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="V11" s="3" t="s">
+      <c r="B11" s="5" t="s">
         <v>33</v>
       </c>
+      <c r="C11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="V11" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="V12" s="3" t="s">
+      <c r="B12" s="5" t="s">
         <v>36</v>
       </c>
+      <c r="C12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="V12" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="V13" s="3" t="s">
+      <c r="C13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="V13" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="V14" s="3" t="s">
+      <c r="C14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="V14" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="V15" s="3" t="s">
+      <c r="C15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="V15" s="4" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="V16" s="3" t="s">
+      <c r="C16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="V16" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="V17" s="3" t="s">
+      <c r="C17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="V17" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="V18" s="3" t="s">
+      <c r="C18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="V18" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="V19" s="3" t="s">
+      <c r="C19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="V19" s="4" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="V20" s="3" t="s">
+      <c r="C20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="V20" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="V21" s="3" t="s">
+      <c r="C21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="V21" s="4" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>